<commit_message>
reconfigured stepper enable pinouts and IO control
-reverted IO control of stepper enable pins to allow multiple enable pins (individual) pins for each stepper since it is need by some controller boards
</commit_message>
<xml_diff>
--- a/docs/avr_mcumap_gen.xlsx
+++ b/docs/avr_mcumap_gen.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JCEM\Documents\GitHub\uCNC\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD2EAB0-290E-47B4-9E0D-716B6CD5B231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF4242A-11BF-4BF5-9C6C-A6022812C64A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="113">
   <si>
     <t>Names</t>
   </si>
@@ -349,6 +349,21 @@
   </si>
   <si>
     <t>STEPPER_ENABLE</t>
+  </si>
+  <si>
+    <t>STEPPER1_ENABLE</t>
+  </si>
+  <si>
+    <t>STEPPER2_ENABLE</t>
+  </si>
+  <si>
+    <t>STEPPER3_ENABLE</t>
+  </si>
+  <si>
+    <t>STEPPER4_ENABLE</t>
+  </si>
+  <si>
+    <t>STEPPER5_ENABLE</t>
   </si>
 </sst>
 </file>
@@ -750,8 +765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E97"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="I98" sqref="I98:I102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -844,7 +859,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="3" t="str">
-        <f t="shared" ref="B3:B97" si="0">"DIO"&amp;A3</f>
+        <f t="shared" ref="B3:B98" si="0">"DIO"&amp;A3</f>
         <v>DIO0</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -6767,7 +6782,7 @@
         <v>0</v>
       </c>
       <c r="E65" s="6" t="str">
-        <f t="shared" ref="E65:E97" si="11">"#if(defined("&amp;C65&amp;"_PORT) &amp;&amp; defined("&amp;C65&amp;"_BIT))
+        <f t="shared" ref="E65:E102" si="11">"#if(defined("&amp;C65&amp;"_PORT) &amp;&amp; defined("&amp;C65&amp;"_BIT))
 #define "&amp;B65&amp;" "&amp;A65&amp;"
 #define "&amp;C65&amp;" "&amp;A65&amp;"
 #define "&amp;B65&amp;"_PORT ("&amp;C65&amp;"_PORT)
@@ -8842,15 +8857,45 @@
       <c r="AB97" s="3"/>
     </row>
     <row r="98" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="1"/>
-      <c r="B98" s="1"/>
-      <c r="C98" s="1"/>
-      <c r="D98" s="1"/>
-      <c r="E98" s="1"/>
+      <c r="A98" s="3">
+        <v>95</v>
+      </c>
+      <c r="B98" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>DIO95</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D98" s="7">
+        <v>1</v>
+      </c>
+      <c r="E98" s="6" t="str">
+        <f t="shared" si="11"/>
+        <v>#if(defined(STEPPER1_ENABLE_PORT) &amp;&amp; defined(STEPPER1_ENABLE_BIT))
+#define DIO95 95
+#define STEPPER1_ENABLE 95
+#define DIO95_PORT (STEPPER1_ENABLE_PORT)
+#define DIO95_BIT (STEPPER1_ENABLE_BIT)
+#define STEPPER1_ENABLE_OUTREG (__outreg__(STEPPER1_ENABLE_PORT))
+#define STEPPER1_ENABLE_INREG (__inreg__(STEPPER1_ENABLE_PORT))
+#define STEPPER1_ENABLE_DIRREG (__dirreg__(STEPPER1_ENABLE_PORT))
+#define DIO95_OUTREG (__outreg__(STEPPER1_ENABLE_PORT))
+#define DIO95_INREG (__inreg__(STEPPER1_ENABLE_PORT))
+#define DIO95_DIRREG (__dirreg__(STEPPER1_ENABLE_PORT))
+#endif</v>
+      </c>
       <c r="F98" s="1"/>
       <c r="G98" s="1"/>
       <c r="H98" s="1"/>
-      <c r="I98" s="1"/>
+      <c r="I98" s="3" t="str">
+        <f t="shared" ref="I98:I102" si="15">"#ifdef "&amp;C98&amp;"
+mcu_config_ouput("&amp;C98&amp;");
+#endif"</f>
+        <v>#ifdef STEPPER1_ENABLE
+mcu_config_ouput(STEPPER1_ENABLE);
+#endif</v>
+      </c>
       <c r="J98" s="1"/>
       <c r="K98" s="1"/>
       <c r="L98" s="1"/>
@@ -8872,15 +8917,43 @@
       <c r="AB98" s="1"/>
     </row>
     <row r="99" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="1"/>
-      <c r="B99" s="1"/>
-      <c r="C99" s="1"/>
-      <c r="D99" s="1"/>
-      <c r="E99" s="1"/>
+      <c r="A99" s="3">
+        <v>96</v>
+      </c>
+      <c r="B99" s="3" t="str">
+        <f t="shared" ref="B99:B102" si="16">"DIO"&amp;A99</f>
+        <v>DIO96</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D99" s="7">
+        <v>2</v>
+      </c>
+      <c r="E99" s="6" t="str">
+        <f t="shared" si="11"/>
+        <v>#if(defined(STEPPER2_ENABLE_PORT) &amp;&amp; defined(STEPPER2_ENABLE_BIT))
+#define DIO96 96
+#define STEPPER2_ENABLE 96
+#define DIO96_PORT (STEPPER2_ENABLE_PORT)
+#define DIO96_BIT (STEPPER2_ENABLE_BIT)
+#define STEPPER2_ENABLE_OUTREG (__outreg__(STEPPER2_ENABLE_PORT))
+#define STEPPER2_ENABLE_INREG (__inreg__(STEPPER2_ENABLE_PORT))
+#define STEPPER2_ENABLE_DIRREG (__dirreg__(STEPPER2_ENABLE_PORT))
+#define DIO96_OUTREG (__outreg__(STEPPER2_ENABLE_PORT))
+#define DIO96_INREG (__inreg__(STEPPER2_ENABLE_PORT))
+#define DIO96_DIRREG (__dirreg__(STEPPER2_ENABLE_PORT))
+#endif</v>
+      </c>
       <c r="F99" s="1"/>
       <c r="G99" s="1"/>
       <c r="H99" s="1"/>
-      <c r="I99" s="1"/>
+      <c r="I99" s="3" t="str">
+        <f t="shared" si="15"/>
+        <v>#ifdef STEPPER2_ENABLE
+mcu_config_ouput(STEPPER2_ENABLE);
+#endif</v>
+      </c>
       <c r="J99" s="1"/>
       <c r="K99" s="1"/>
       <c r="L99" s="1"/>
@@ -8902,15 +8975,43 @@
       <c r="AB99" s="1"/>
     </row>
     <row r="100" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="1"/>
-      <c r="B100" s="1"/>
-      <c r="C100" s="1"/>
-      <c r="D100" s="1"/>
-      <c r="E100" s="1"/>
+      <c r="A100" s="3">
+        <v>97</v>
+      </c>
+      <c r="B100" s="3" t="str">
+        <f t="shared" si="16"/>
+        <v>DIO97</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D100" s="7">
+        <v>3</v>
+      </c>
+      <c r="E100" s="6" t="str">
+        <f t="shared" si="11"/>
+        <v>#if(defined(STEPPER3_ENABLE_PORT) &amp;&amp; defined(STEPPER3_ENABLE_BIT))
+#define DIO97 97
+#define STEPPER3_ENABLE 97
+#define DIO97_PORT (STEPPER3_ENABLE_PORT)
+#define DIO97_BIT (STEPPER3_ENABLE_BIT)
+#define STEPPER3_ENABLE_OUTREG (__outreg__(STEPPER3_ENABLE_PORT))
+#define STEPPER3_ENABLE_INREG (__inreg__(STEPPER3_ENABLE_PORT))
+#define STEPPER3_ENABLE_DIRREG (__dirreg__(STEPPER3_ENABLE_PORT))
+#define DIO97_OUTREG (__outreg__(STEPPER3_ENABLE_PORT))
+#define DIO97_INREG (__inreg__(STEPPER3_ENABLE_PORT))
+#define DIO97_DIRREG (__dirreg__(STEPPER3_ENABLE_PORT))
+#endif</v>
+      </c>
       <c r="F100" s="1"/>
       <c r="G100" s="1"/>
       <c r="H100" s="1"/>
-      <c r="I100" s="1"/>
+      <c r="I100" s="3" t="str">
+        <f t="shared" si="15"/>
+        <v>#ifdef STEPPER3_ENABLE
+mcu_config_ouput(STEPPER3_ENABLE);
+#endif</v>
+      </c>
       <c r="J100" s="1"/>
       <c r="K100" s="1"/>
       <c r="L100" s="1"/>
@@ -8932,15 +9033,43 @@
       <c r="AB100" s="1"/>
     </row>
     <row r="101" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="1"/>
-      <c r="B101" s="1"/>
-      <c r="C101" s="1"/>
-      <c r="D101" s="1"/>
-      <c r="E101" s="1"/>
+      <c r="A101" s="3">
+        <v>98</v>
+      </c>
+      <c r="B101" s="3" t="str">
+        <f t="shared" si="16"/>
+        <v>DIO98</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D101" s="7">
+        <v>4</v>
+      </c>
+      <c r="E101" s="6" t="str">
+        <f t="shared" si="11"/>
+        <v>#if(defined(STEPPER4_ENABLE_PORT) &amp;&amp; defined(STEPPER4_ENABLE_BIT))
+#define DIO98 98
+#define STEPPER4_ENABLE 98
+#define DIO98_PORT (STEPPER4_ENABLE_PORT)
+#define DIO98_BIT (STEPPER4_ENABLE_BIT)
+#define STEPPER4_ENABLE_OUTREG (__outreg__(STEPPER4_ENABLE_PORT))
+#define STEPPER4_ENABLE_INREG (__inreg__(STEPPER4_ENABLE_PORT))
+#define STEPPER4_ENABLE_DIRREG (__dirreg__(STEPPER4_ENABLE_PORT))
+#define DIO98_OUTREG (__outreg__(STEPPER4_ENABLE_PORT))
+#define DIO98_INREG (__inreg__(STEPPER4_ENABLE_PORT))
+#define DIO98_DIRREG (__dirreg__(STEPPER4_ENABLE_PORT))
+#endif</v>
+      </c>
       <c r="F101" s="1"/>
       <c r="G101" s="1"/>
       <c r="H101" s="1"/>
-      <c r="I101" s="1"/>
+      <c r="I101" s="3" t="str">
+        <f t="shared" si="15"/>
+        <v>#ifdef STEPPER4_ENABLE
+mcu_config_ouput(STEPPER4_ENABLE);
+#endif</v>
+      </c>
       <c r="J101" s="1"/>
       <c r="K101" s="1"/>
       <c r="L101" s="1"/>
@@ -8962,15 +9091,43 @@
       <c r="AB101" s="1"/>
     </row>
     <row r="102" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="1"/>
-      <c r="B102" s="1"/>
-      <c r="C102" s="1"/>
-      <c r="D102" s="1"/>
-      <c r="E102" s="1"/>
+      <c r="A102" s="3">
+        <v>99</v>
+      </c>
+      <c r="B102" s="3" t="str">
+        <f t="shared" si="16"/>
+        <v>DIO99</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D102" s="7">
+        <v>5</v>
+      </c>
+      <c r="E102" s="6" t="str">
+        <f t="shared" si="11"/>
+        <v>#if(defined(STEPPER5_ENABLE_PORT) &amp;&amp; defined(STEPPER5_ENABLE_BIT))
+#define DIO99 99
+#define STEPPER5_ENABLE 99
+#define DIO99_PORT (STEPPER5_ENABLE_PORT)
+#define DIO99_BIT (STEPPER5_ENABLE_BIT)
+#define STEPPER5_ENABLE_OUTREG (__outreg__(STEPPER5_ENABLE_PORT))
+#define STEPPER5_ENABLE_INREG (__inreg__(STEPPER5_ENABLE_PORT))
+#define STEPPER5_ENABLE_DIRREG (__dirreg__(STEPPER5_ENABLE_PORT))
+#define DIO99_OUTREG (__outreg__(STEPPER5_ENABLE_PORT))
+#define DIO99_INREG (__inreg__(STEPPER5_ENABLE_PORT))
+#define DIO99_DIRREG (__dirreg__(STEPPER5_ENABLE_PORT))
+#endif</v>
+      </c>
       <c r="F102" s="1"/>
       <c r="G102" s="1"/>
       <c r="H102" s="1"/>
-      <c r="I102" s="1"/>
+      <c r="I102" s="3" t="str">
+        <f t="shared" si="15"/>
+        <v>#ifdef STEPPER5_ENABLE
+mcu_config_ouput(STEPPER5_ENABLE);
+#endif</v>
+      </c>
       <c r="J102" s="1"/>
       <c r="K102" s="1"/>
       <c r="L102" s="1"/>

</xml_diff>